<commit_message>
Backlog 8 and Retrospective 7 + updated the week number of Backlog week 7 (since it said week 6 before)
</commit_message>
<xml_diff>
--- a/doc/Scrum/Backlogs/Backlog Week 7.xlsx
+++ b/doc/Scrum/Backlogs/Backlog Week 7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\template\doc\Scrum\Backlogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B176670-A255-47C7-94B3-2902E2DCD570}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABF351C-14A4-45BD-B6D2-B7D37895F2B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DB0F79B-32C8-42B6-AA2D-DE25723E6E6C}"/>
   </bookViews>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Iteration</t>
-  </si>
-  <si>
-    <t>Week 6</t>
   </si>
   <si>
     <t>Project</t>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>I am a user and i want to be able to access my co2 score from the internet</t>
+  </si>
+  <si>
+    <t>Week 7</t>
   </si>
 </sst>
 </file>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD89F68-06D4-4C93-BEBE-52971817F0FB}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B30" sqref="B23:B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="9"/>
@@ -739,10 +739,10 @@
     <row r="4" spans="1:26">
       <c r="A4" s="1"/>
       <c r="B4" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -771,10 +771,10 @@
     <row r="5" spans="1:26">
       <c r="A5" s="1"/>
       <c r="B5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -859,7 +859,7 @@
     <row r="8" spans="1:26" ht="22.8">
       <c r="A8" s="1"/>
       <c r="B8" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -917,7 +917,7 @@
     <row r="10" spans="1:26" ht="18.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="18">
         <v>6</v>
@@ -949,10 +949,10 @@
     <row r="11" spans="1:26" ht="20.25" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
@@ -1009,22 +1009,22 @@
     <row r="13" spans="1:26" ht="34.5" customHeight="1" thickBot="1">
       <c r="A13" s="1"/>
       <c r="B13" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="D13" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="E13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="F13" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="G13" s="20" t="s">
         <v>15</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>16</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1049,22 +1049,22 @@
     <row r="14" spans="1:26" ht="40.200000000000003" thickTop="1">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" s="4">
         <v>4</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1089,22 +1089,22 @@
     <row r="15" spans="1:26" ht="52.8">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="4">
         <v>4</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1129,22 +1129,22 @@
     <row r="16" spans="1:26" ht="26.4">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="4">
         <v>4</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1169,22 +1169,22 @@
     <row r="17" spans="1:26" ht="39.6">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" s="4">
         <v>4</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1209,22 +1209,22 @@
     <row r="18" spans="1:26" ht="52.8">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F18" s="4">
         <v>4</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1249,22 +1249,22 @@
     <row r="19" spans="1:26" ht="26.4">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F19" s="4">
         <v>4</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>

</xml_diff>

<commit_message>
Revert "Merge remote-tracking branch 'origin/Testing_LoginPackage' into Final_Report"
This reverts commit 7930f2c4b560e059a23b8208094ae02c58882e47
</commit_message>
<xml_diff>
--- a/doc/Scrum/Backlogs/Backlog Week 7.xlsx
+++ b/doc/Scrum/Backlogs/Backlog Week 7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\template\doc\Scrum\Backlogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABF351C-14A4-45BD-B6D2-B7D37895F2B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B176670-A255-47C7-94B3-2902E2DCD570}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DB0F79B-32C8-42B6-AA2D-DE25723E6E6C}"/>
   </bookViews>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Iteration</t>
+  </si>
+  <si>
+    <t>Week 6</t>
   </si>
   <si>
     <t>Project</t>
@@ -139,9 +142,6 @@
   </si>
   <si>
     <t>I am a user and i want to be able to access my co2 score from the internet</t>
-  </si>
-  <si>
-    <t>Week 7</t>
   </si>
 </sst>
 </file>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD89F68-06D4-4C93-BEBE-52971817F0FB}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B30" sqref="B23:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="9"/>
@@ -739,10 +739,10 @@
     <row r="4" spans="1:26">
       <c r="A4" s="1"/>
       <c r="B4" s="11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -771,10 +771,10 @@
     <row r="5" spans="1:26">
       <c r="A5" s="1"/>
       <c r="B5" s="11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -859,7 +859,7 @@
     <row r="8" spans="1:26" ht="22.8">
       <c r="A8" s="1"/>
       <c r="B8" s="16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -917,7 +917,7 @@
     <row r="10" spans="1:26" ht="18.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="18">
         <v>6</v>
@@ -949,10 +949,10 @@
     <row r="11" spans="1:26" ht="20.25" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
@@ -1009,22 +1009,22 @@
     <row r="13" spans="1:26" ht="34.5" customHeight="1" thickBot="1">
       <c r="A13" s="1"/>
       <c r="B13" s="20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1049,22 +1049,22 @@
     <row r="14" spans="1:26" ht="40.200000000000003" thickTop="1">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F14" s="4">
         <v>4</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1089,22 +1089,22 @@
     <row r="15" spans="1:26" ht="52.8">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F15" s="4">
         <v>4</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1129,22 +1129,22 @@
     <row r="16" spans="1:26" ht="26.4">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="D16" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F16" s="4">
         <v>4</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1169,22 +1169,22 @@
     <row r="17" spans="1:26" ht="39.6">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F17" s="4">
         <v>4</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1209,22 +1209,22 @@
     <row r="18" spans="1:26" ht="52.8">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F18" s="4">
         <v>4</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1249,22 +1249,22 @@
     <row r="19" spans="1:26" ht="26.4">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F19" s="4">
         <v>4</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge remote-tracking branch 'origin/Testing_LoginPackage' into Final_Report""
This reverts commit 8fdf320cfca07e85857fb79bd1c4a376166cc099
</commit_message>
<xml_diff>
--- a/doc/Scrum/Backlogs/Backlog Week 7.xlsx
+++ b/doc/Scrum/Backlogs/Backlog Week 7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\template\doc\Scrum\Backlogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B176670-A255-47C7-94B3-2902E2DCD570}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DABF351C-14A4-45BD-B6D2-B7D37895F2B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0DB0F79B-32C8-42B6-AA2D-DE25723E6E6C}"/>
   </bookViews>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Iteration</t>
-  </si>
-  <si>
-    <t>Week 6</t>
   </si>
   <si>
     <t>Project</t>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>I am a user and i want to be able to access my co2 score from the internet</t>
+  </si>
+  <si>
+    <t>Week 7</t>
   </si>
 </sst>
 </file>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD89F68-06D4-4C93-BEBE-52971817F0FB}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B30" sqref="B23:B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="9"/>
@@ -739,10 +739,10 @@
     <row r="4" spans="1:26">
       <c r="A4" s="1"/>
       <c r="B4" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -771,10 +771,10 @@
     <row r="5" spans="1:26">
       <c r="A5" s="1"/>
       <c r="B5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -859,7 +859,7 @@
     <row r="8" spans="1:26" ht="22.8">
       <c r="A8" s="1"/>
       <c r="B8" s="16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -917,7 +917,7 @@
     <row r="10" spans="1:26" ht="18.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="18">
         <v>6</v>
@@ -949,10 +949,10 @@
     <row r="11" spans="1:26" ht="20.25" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
@@ -1009,22 +1009,22 @@
     <row r="13" spans="1:26" ht="34.5" customHeight="1" thickBot="1">
       <c r="A13" s="1"/>
       <c r="B13" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="D13" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="E13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="F13" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="G13" s="20" t="s">
         <v>15</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>16</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1049,22 +1049,22 @@
     <row r="14" spans="1:26" ht="40.200000000000003" thickTop="1">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F14" s="4">
         <v>4</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1089,22 +1089,22 @@
     <row r="15" spans="1:26" ht="52.8">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" s="4">
         <v>4</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1129,22 +1129,22 @@
     <row r="16" spans="1:26" ht="26.4">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="4">
         <v>4</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1169,22 +1169,22 @@
     <row r="17" spans="1:26" ht="39.6">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" s="4">
         <v>4</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1209,22 +1209,22 @@
     <row r="18" spans="1:26" ht="52.8">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F18" s="4">
         <v>4</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1249,22 +1249,22 @@
     <row r="19" spans="1:26" ht="26.4">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F19" s="4">
         <v>4</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>

</xml_diff>